<commit_message>
upload lịch sử trading
</commit_message>
<xml_diff>
--- a/Tiếng Trung/Từ mới.xlsx
+++ b/Tiếng Trung/Từ mới.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D246B8F8-20E0-4B7A-A644-F746384DA1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607C9F9C-D7FC-415F-A6D5-2FE39D5CE556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -453,9 +454,6 @@
     <t>差不多</t>
   </si>
   <si>
-    <t xml:space="preserve">gần như, gần đủ </t>
-  </si>
-  <si>
     <t>拒绝</t>
   </si>
   <si>
@@ -2431,6 +2429,9 @@
   </si>
   <si>
     <t>day du?, tron ven., thoai? Mai'</t>
+  </si>
+  <si>
+    <t>gần như, gần đủ, tương đối</t>
   </si>
 </sst>
 </file>
@@ -2757,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q146" sqref="Q146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="30.6" x14ac:dyDescent="0.55000000000000004"/>
@@ -2848,7 +2849,7 @@
         <v>21</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.55000000000000004">
@@ -3080,7 +3081,7 @@
         <v>81</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.55000000000000004">
@@ -3305,2434 +3306,2434 @@
         <v>139</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>140</v>
+        <v>799</v>
       </c>
     </row>
     <row r="54" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D54" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="Q54" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="Q54" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="55" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="Q55" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="Q55" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="56" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D56" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="Q56" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="57" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="Q57" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="58" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="Q58" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="59" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="Q59" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="60" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D60" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="Q60" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="61" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="Q61" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="62" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D62" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="Q62" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="63" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="Q63" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="64" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="Q64" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="Q64" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="Q65" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="Q65" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="Q66" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="Q66" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D67" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G67" s="1" t="s">
+      <c r="Q67" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="Q67" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D68" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="Q68" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="Q68" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D69" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="Q69" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="Q69" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D70" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="Q70" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="Q70" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D71" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="Q71" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="Q71" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D72" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q72" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="Q72" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D73" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="Q73" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="Q73" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D74" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="Q74" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D75" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G75" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q75" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="Q75" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D76" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="Q76" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q76" s="1" t="s">
+      <c r="W76" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="W76" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D77" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="Q77" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="Q77" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D78" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="Q78" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D79" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D81" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="Q81" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="Q81" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="82" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D82" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="Q82" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="Q82" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="83" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D83" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="Q83" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="Q83" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="84" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D84" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G84" s="1" t="s">
+      <c r="Q84" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="Q84" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="85" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D85" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="Q85" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="Q85" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="86" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D86" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="Q86" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="Q86" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="87" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D87" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="Q87" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="Q87" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="88" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D88" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G88" s="1" t="s">
+      <c r="Q88" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="Q88" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="89" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D89" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="Q89" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="Q89" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="90" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D90" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G90" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G90" s="1" t="s">
+      <c r="Q90" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="Q90" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="91" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D91" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q91" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="Q91" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="92" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D92" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="Q92" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="Q92" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="93" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D93" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G93" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G93" s="1" t="s">
+      <c r="Q93" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="Q93" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="94" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D94" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G94" s="1" t="s">
+      <c r="Q94" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="Q94" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="95" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D95" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G95" s="1" t="s">
+      <c r="Q95" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="Q95" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="96" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D96" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G96" s="1" t="s">
+      <c r="Q96" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="Q96" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="97" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D97" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="Q97" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="Q97" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="98" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D98" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G98" s="1" t="s">
+      <c r="Q98" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="Q98" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="99" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D99" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="Q99" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="Q99" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="100" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D100" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G100" s="1" t="s">
+      <c r="Q100" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="Q100" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="101" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D101" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="Q101" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="Q101" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="102" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D102" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G102" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G102" s="1" t="s">
+      <c r="Q102" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="Q102" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="103" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D103" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q103" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="104" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D104" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="Q104" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="Q104" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="105" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D105" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q105" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="Q105" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="106" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D106" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G106" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G106" s="1" t="s">
+      <c r="Q106" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="Q106" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="107" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D107" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="Q107" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="Q107" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="108" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D108" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G108" s="1" t="s">
+      <c r="Q108" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="109" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D109" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G109" s="1" t="s">
+      <c r="Q109" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="Q109" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="110" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D110" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="G110" s="1" t="s">
+      <c r="Q110" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="Q110" s="1" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="111" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D111" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G111" s="1" t="s">
+      <c r="Q111" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="Q111" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="112" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D112" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="G112" s="1" t="s">
+      <c r="Q112" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="Q112" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="113" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D113" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G113" s="1" t="s">
+      <c r="Q113" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="Q113" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="114" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D114" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="Q114" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="Q114" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="115" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D115" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="Q115" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="Q115" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="116" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D116" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="G116" s="1" t="s">
+      <c r="Q116" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="Q116" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="117" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D117" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="Q117" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="Q117" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="118" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D118" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G118" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G118" s="1" t="s">
+      <c r="Q118" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="Q118" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="119" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D119" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="G119" s="1" t="s">
+      <c r="Q119" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="Q119" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="120" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D120" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="G120" s="1" t="s">
+      <c r="Q120" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="Q120" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="121" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D121" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="Q121" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="Q121" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="122" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D122" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="G122" s="1" t="s">
+      <c r="Q122" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="Q122" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="123" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D123" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="G123" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="Q123" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="124" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D124" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G124" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="G124" s="1" t="s">
+      <c r="Q124" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="Q124" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="125" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D125" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G125" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="G125" s="1" t="s">
+      <c r="Q125" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="Q125" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="126" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D126" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G126" s="1" t="s">
+      <c r="Q126" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="Q126" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="127" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D127" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G127" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="G127" s="1" t="s">
+      <c r="Q127" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="Q127" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="128" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D128" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q128" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="Q128" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="129" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D129" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="G129" s="1" t="s">
+      <c r="Q129" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="Q129" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="130" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D130" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G130" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="Q130" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="Q130" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="131" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D131" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G131" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="Q131" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="Q131" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="132" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D132" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="Q132" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="Q132" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="133" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D133" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="Q133" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="Q133" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="134" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D134" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="Q134" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="Q134" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="135" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D135" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G135" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="G135" s="1" t="s">
+      <c r="Q135" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="Q135" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="136" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D136" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G136" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="G136" s="1" t="s">
+      <c r="Q136" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="Q136" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="137" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D137" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G137" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="G137" s="1" t="s">
+      <c r="Q137" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="138" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D138" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="G138" s="1" t="s">
+      <c r="Q138" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="Q138" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="139" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D139" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="G139" s="1" t="s">
+      <c r="Q139" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="Q139" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="140" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D140" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="G140" s="1" t="s">
+      <c r="Q140" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="Q140" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="141" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D141" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="G141" s="1" t="s">
+      <c r="Q141" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="Q141" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="142" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D142" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G142" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G142" s="1" t="s">
+      <c r="Q142" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="Q142" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="143" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D143" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G143" s="1" t="s">
+      <c r="Q143" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="Q143" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="144" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D144" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q144" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="Q144" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="145" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D145" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="G145" s="1" t="s">
+      <c r="Q145" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="Q145" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="146" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D146" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="G146" s="1" t="s">
+      <c r="Q146" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="Q146" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="147" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D147" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="Q147" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="Q147" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="148" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D148" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="149" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D149" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="Q149" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="Q149" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="150" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D150" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G150" s="1" t="s">
+      <c r="Q150" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="151" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D151" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G151" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="G151" s="1" t="s">
+      <c r="Q151" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="Q151" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="152" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D152" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="G152" s="1" t="s">
+      <c r="Q152" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="Q152" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="153" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D153" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="G153" s="1" t="s">
+      <c r="Q153" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="Q153" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="154" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D154" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G154" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G154" s="1" t="s">
+      <c r="Q154" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="Q154" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="155" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D155" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G155" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="G155" s="1" t="s">
+      <c r="Q155" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="Q155" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="156" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D156" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q156" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="Q156" s="1" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="157" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D157" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="G157" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="G157" s="1" t="s">
+      <c r="Q157" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="Q157" s="1" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="158" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D158" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G158" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="G158" s="1" t="s">
+      <c r="Q158" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="Q158" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="159" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D159" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G159" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="G159" s="1" t="s">
+      <c r="Q159" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="160" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D160" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="G160" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="Q160" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D161" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G161" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G161" s="1" t="s">
+      <c r="Q161" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="Q161" s="1" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D162" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="G162" s="1" t="s">
+      <c r="Q162" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="Q162" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D163" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G163" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="G163" s="1" t="s">
+      <c r="Q163" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="Q163" s="1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D164" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G164" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G164" s="1" t="s">
+      <c r="Q164" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="Q164" s="1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D165" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G165" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="G165" s="1" t="s">
+      <c r="Q165" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="Q165" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D166" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q166" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="Q166" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D167" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G167" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="G167" s="1" t="s">
+      <c r="Q167" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="Q167" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D168" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G168" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G168" s="1" t="s">
+      <c r="Q168" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="Q168" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D169" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G169" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="G169" s="1" t="s">
+      <c r="Q169" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="Q169" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D170" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q170" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q170" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D172" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G172" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="G172" s="1" t="s">
+      <c r="Q172" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="Q172" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D173" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="G173" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="G173" s="1" t="s">
+      <c r="Q173" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="Q173" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D174" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G174" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="G174" s="1" t="s">
+      <c r="Q174" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="Q174" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D175" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q175" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="Q175" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D176" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="G176" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="G176" s="1" t="s">
-        <v>496</v>
-      </c>
       <c r="Q176" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="177" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D177" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="G177" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="G177" s="1" t="s">
+      <c r="Q177" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="Q177" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="178" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D178" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="G178" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="G178" s="1" t="s">
+      <c r="Q178" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="Q178" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="179" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D179" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G179" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="G179" s="1" t="s">
+      <c r="Q179" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="Q179" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="180" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D180" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G180" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="G180" s="1" t="s">
+      <c r="Q180" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="Q180" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="181" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D181" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G181" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="G181" s="1" t="s">
+      <c r="Q181" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="Q181" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="182" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D182" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="G182" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="G182" s="1" t="s">
+      <c r="Q182" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="Q182" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="183" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D183" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G183" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="G183" s="1" t="s">
+      <c r="Q183" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="Q183" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="184" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D184" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="G184" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="G184" s="1" t="s">
+      <c r="Q184" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="Q184" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="185" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D185" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="G185" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="G185" s="1" t="s">
+      <c r="Q185" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="Q185" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="186" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D186" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="G186" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="G186" s="1" t="s">
+      <c r="Q186" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="Q186" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="187" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D187" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G187" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="G187" s="1" t="s">
+      <c r="Q187" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="Q187" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="188" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D188" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G188" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G188" s="1" t="s">
+      <c r="Q188" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="Q188" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="189" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D189" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="G189" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="G189" s="1" t="s">
+      <c r="Q189" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="Q189" s="1" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="190" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D190" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="G190" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="G190" s="1" t="s">
+      <c r="Q190" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="Q190" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="191" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D191" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G191" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="G191" s="1" t="s">
+      <c r="Q191" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="Q191" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="192" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D192" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="G192" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="G192" s="1" t="s">
+      <c r="Q192" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="Q192" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="193" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D193" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="G193" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="G193" s="1" t="s">
+      <c r="Q193" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="Q193" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="194" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D194" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G194" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="G194" s="1" t="s">
+      <c r="Q194" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="Q194" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="195" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D195" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="G195" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="G195" s="1" t="s">
+      <c r="Q195" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="Q195" s="1" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="196" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D196" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G196" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="G196" s="1" t="s">
+      <c r="Q196" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="Q196" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="197" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D197" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="G197" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="G197" s="1" t="s">
+      <c r="Q197" s="1" t="s">
         <v>559</v>
-      </c>
-      <c r="Q197" s="1" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="198" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D198" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q198" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="Q198" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="199" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D199" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="G199" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="G199" s="1" t="s">
-        <v>564</v>
-      </c>
       <c r="Q199" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="200" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D200" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G200" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="G200" s="1" t="s">
+      <c r="Q200" s="1" t="s">
         <v>566</v>
-      </c>
-      <c r="Q200" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="201" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D201" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G201" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="G201" s="1" t="s">
+      <c r="Q201" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="Q201" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="202" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D202" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G202" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="G202" s="1" t="s">
+      <c r="Q202" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="Q202" s="1" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="203" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D203" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G203" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="G203" s="1" t="s">
+      <c r="Q203" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="Q203" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="204" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D204" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="G204" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="G204" s="1" t="s">
+      <c r="Q204" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="Q204" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="205" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D205" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="G205" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="G205" s="1" t="s">
+      <c r="Q205" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="Q205" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="206" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D206" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G206" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q206" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="Q206" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="207" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D207" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="G207" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="G207" s="1" t="s">
+      <c r="Q207" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="Q207" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="208" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D208" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q208" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="Q208" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="209" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D209" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="G209" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="G209" s="1" t="s">
+      <c r="Q209" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="Q209" s="1" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="210" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D210" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="G210" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="G210" s="1" t="s">
+      <c r="Q210" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="Q210" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="211" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D211" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="G211" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="G211" s="1" t="s">
+      <c r="Q211" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="Q211" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="212" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D212" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="G212" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="G212" s="1" t="s">
+      <c r="Q212" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="Q212" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="213" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D213" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="G213" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="G213" s="1" t="s">
+      <c r="Q213" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="Q213" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="214" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D214" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="G214" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="G214" s="1" t="s">
+      <c r="Q214" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="Q214" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="215" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D215" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="G215" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="G215" s="1" t="s">
+      <c r="Q215" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="Q215" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="216" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D216" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="G216" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G216" s="1" t="s">
+      <c r="Q216" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="Q216" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="217" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D217" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q217" s="1" t="s">
         <v>615</v>
-      </c>
-      <c r="Q217" s="1" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="218" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D218" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="G218" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="G218" s="1" t="s">
+      <c r="Q218" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="Q218" s="1" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="219" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D219" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="G219" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="G219" s="1" t="s">
+      <c r="Q219" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="Q219" s="1" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="220" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D220" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G220" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="G220" s="1" t="s">
+      <c r="Q220" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="Q220" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="221" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D221" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="G221" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="G221" s="1" t="s">
+      <c r="Q221" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="Q221" s="1" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="222" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D222" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="G222" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="G222" s="1" t="s">
+      <c r="Q222" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="Q222" s="1" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="223" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D223" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="G223" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="G223" s="1" t="s">
+      <c r="Q223" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="Q223" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="224" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D224" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="G224" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="G224" s="1" t="s">
+      <c r="Q224" s="1" t="s">
         <v>636</v>
-      </c>
-      <c r="Q224" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="225" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D225" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="G225" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="G225" s="1" t="s">
+      <c r="Q225" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="Q225" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="226" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D226" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="G226" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="G226" s="1" t="s">
+      <c r="Q226" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="Q226" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="227" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D227" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="G227" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="Q227" s="1" t="s">
         <v>644</v>
-      </c>
-      <c r="G227" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="Q227" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="228" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D228" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="G228" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="G228" s="1" t="s">
+      <c r="Q228" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="Q228" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="229" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D229" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="G229" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="G229" s="1" t="s">
+      <c r="Q229" s="1" t="s">
         <v>651</v>
-      </c>
-      <c r="Q229" s="1" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="230" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D230" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="G230" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="G230" s="1" t="s">
+      <c r="Q230" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="Q230" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="231" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D231" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="G231" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="G231" s="1" t="s">
-        <v>657</v>
-      </c>
       <c r="Q231" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="232" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D232" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="G232" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="G232" s="1" t="s">
-        <v>659</v>
-      </c>
       <c r="Q232" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="233" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D233" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="G233" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="G233" s="1" t="s">
+      <c r="Q233" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="Q233" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="234" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D234" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="G234" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="G234" s="1" t="s">
+      <c r="Q234" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="Q234" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="235" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D235" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G235" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="G235" s="1" t="s">
+      <c r="Q235" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="Q235" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="236" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D236" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G236" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="G236" s="1" t="s">
+      <c r="Q236" s="1" t="s">
         <v>672</v>
-      </c>
-      <c r="Q236" s="1" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="237" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D237" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="G237" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="G237" s="1" t="s">
-        <v>675</v>
-      </c>
       <c r="Q237" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="238" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D238" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="G238" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="G238" s="1" t="s">
+      <c r="Q238" s="1" t="s">
         <v>677</v>
-      </c>
-      <c r="Q238" s="1" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="239" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D239" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="G239" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="G239" s="1" t="s">
+      <c r="Q239" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="Q239" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="240" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D240" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="G240" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="G240" s="1" t="s">
+      <c r="Q240" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="Q240" s="1" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="241" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D241" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="G241" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="G241" s="1" t="s">
-        <v>687</v>
-      </c>
       <c r="Q241" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="242" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D242" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="G242" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="G242" s="1" t="s">
+      <c r="Q242" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="Q242" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="243" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D243" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="G243" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="G243" s="1" t="s">
+      <c r="Q243" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="Q243" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="244" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D244" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="G244" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="G244" s="1" t="s">
+      <c r="Q244" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="Q244" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="245" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D245" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="G245" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="G245" s="1" t="s">
+      <c r="Q245" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="Q245" s="1" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="246" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D246" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="G246" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="G246" s="1" t="s">
+      <c r="Q246" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="Q246" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="247" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D247" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="G247" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="G247" s="1" t="s">
+      <c r="Q247" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="Q247" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="248" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D248" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="G248" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="G248" s="1" t="s">
+      <c r="Q248" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="Q248" s="1" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="249" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D249" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="G249" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="G249" s="1" t="s">
+      <c r="Q249" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="Q249" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="250" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D250" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="G250" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="G250" s="1" t="s">
+      <c r="Q250" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="Q250" s="1" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="251" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D251" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="G251" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="G251" s="1" t="s">
+      <c r="Q251" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="Q251" s="1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="252" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D252" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="G252" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="G252" s="1" t="s">
+      <c r="Q252" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="Q252" s="1" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="253" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D253" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="Q253" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="G253" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="Q253" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="254" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D254" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="G254" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="G254" s="1" t="s">
+      <c r="Q254" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="Q254" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="255" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D255" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="G255" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="G255" s="1" t="s">
+      <c r="Q255" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="Q255" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="256" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D256" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="G256" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="G256" s="1" t="s">
+      <c r="Q256" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="Q256" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="257" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D257" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="G257" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="G257" s="1" t="s">
+      <c r="Q257" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="Q257" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="258" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D258" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="G258" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="G258" s="1" t="s">
+      <c r="Q258" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="Q258" s="1" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="259" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D259" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="G259" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="G259" s="1" t="s">
+      <c r="Q259" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="Q259" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="260" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D260" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="G260" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="G260" s="1" t="s">
+      <c r="Q260" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="Q260" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="261" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D261" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="G261" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="G261" s="1" t="s">
+      <c r="Q261" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="Q261" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="262" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D262" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="G262" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="G262" s="1" t="s">
+      <c r="Q262" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="Q262" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="263" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D263" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="G263" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="G263" s="1" t="s">
-        <v>753</v>
-      </c>
       <c r="Q263" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="264" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D264" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="G264" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="G264" s="1" t="s">
+      <c r="Q264" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="Q264" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="265" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D265" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="G265" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="G265" s="1" t="s">
+      <c r="Q265" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="Q265" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="266" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D266" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="G266" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="G266" s="1" t="s">
+      <c r="Q266" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="Q266" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="267" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D267" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="G267" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="G267" s="1" t="s">
+      <c r="Q267" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="Q267" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="268" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D268" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="G268" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="G268" s="1" t="s">
+      <c r="Q268" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="Q268" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="269" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D269" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="G269" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="G269" s="1" t="s">
+      <c r="Q269" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="Q269" s="1" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="270" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D270" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="G270" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="G270" s="1" t="s">
+      <c r="Q270" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="Q270" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="271" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D271" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="G271" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="G271" s="1" t="s">
+      <c r="Q271" s="1" t="s">
         <v>776</v>
-      </c>
-      <c r="Q271" s="1" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="272" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D272" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="G272" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="G272" s="1" t="s">
+      <c r="Q272" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="Q272" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="273" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D273" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="G273" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="G273" s="1" t="s">
+      <c r="Q273" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="Q273" s="1" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="274" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D274" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="G274" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="G274" s="1" t="s">
+      <c r="Q274" s="1" t="s">
         <v>785</v>
-      </c>
-      <c r="Q274" s="1" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="275" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D275" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="G275" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="G275" s="1" t="s">
+      <c r="Q275" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="Q275" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="276" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D276" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="G276" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="G276" s="1" t="s">
+      <c r="Q276" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="Q276" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="277" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D277" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="G277" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="G277" s="1" t="s">
+      <c r="Q277" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="Q277" s="1" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="278" spans="4:17" x14ac:dyDescent="0.55000000000000004">
       <c r="D278" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="G278" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="G278" s="1" t="s">
+      <c r="Q278" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="Q278" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>